<commit_message>
Made updates to ig questionnaires
</commit_message>
<xml_diff>
--- a/vbai-fhir/CodeSystem-marital-status.xlsx
+++ b/vbai-fhir/CodeSystem-marital-status.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>Property</t>
   </si>
@@ -114,7 +114,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>7</t>
+    <t>10</t>
   </si>
   <si>
     <t>Level</t>
@@ -141,7 +141,7 @@
     <t>RL</t>
   </si>
   <si>
-    <t>In a relationship, not married, living with partner</t>
+    <t>In a relationship, not married, living with partner (Domestic Partner)</t>
   </si>
   <si>
     <t>RNL</t>
@@ -159,19 +159,37 @@
     <t>SD</t>
   </si>
   <si>
-    <t>Separated</t>
+    <t>Legally Separated</t>
   </si>
   <si>
     <t>S</t>
   </si>
   <si>
-    <t>Single</t>
+    <t>Never Married</t>
   </si>
   <si>
     <t>W</t>
   </si>
   <si>
     <t>Widowed</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Annuled</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Interlocutory</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Polygamous</t>
   </si>
 </sst>
 </file>
@@ -474,7 +492,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -578,6 +596,42 @@
       </c>
       <c r="D8" s="2"/>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>